<commit_message>
trend_locations.xlsx updated; misc_emission_analysis now saves line density files with location indicies in the names
</commit_message>
<xml_diff>
--- a/Workspaces/SiteData/trend_locations.xlsx
+++ b/Workspaces/SiteData/trend_locations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="988" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="988"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -1157,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A56" sqref="A54:A56"/>
     </sheetView>
   </sheetViews>
@@ -2817,7 +2817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated trend_locations.xlsx and added ability to merge line density files
trend_locations.xlsx: remove some sites that just weren't going to work,
added Austin, Baltimore, and Cheyenne, and updated the wind reject directions
and some of the box sizes based on the all-winds sectors data.
</commit_message>
<xml_diff>
--- a/Workspaces/SiteData/trend_locations.xlsx
+++ b/Workspaces/SiteData/trend_locations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="220">
   <si>
     <t>Location</t>
   </si>
@@ -311,12 +311,6 @@
     <t>Tucson</t>
   </si>
   <si>
-    <t>Vancouver, BC</t>
-  </si>
-  <si>
-    <t>Vancouver</t>
-  </si>
-  <si>
     <t>Washington, DC</t>
   </si>
   <si>
@@ -437,12 +431,6 @@
     <t>Leland Olds</t>
   </si>
   <si>
-    <t>Marshall, NC</t>
-  </si>
-  <si>
-    <t>Marshall</t>
-  </si>
-  <si>
     <t>Navajo Generating Station, AZ</t>
   </si>
   <si>
@@ -554,24 +542,6 @@
     <t>[0.75 1.5 0.75 0.75]</t>
   </si>
   <si>
-    <t>Can't tell, need to use detail reject</t>
-  </si>
-  <si>
-    <t>The center may be off, there's high NO2 columns in weird places</t>
-  </si>
-  <si>
-    <t>Kind of ambiguous, there's high columns that may be adjacent cities</t>
-  </si>
-  <si>
-    <t>Center seems off</t>
-  </si>
-  <si>
-    <t>May need to be bigger, may be tricked by the large colorbar range</t>
-  </si>
-  <si>
-    <t>May need adjusted, center may be off</t>
-  </si>
-  <si>
     <t>BoxSize</t>
   </si>
   <si>
@@ -593,21 +563,12 @@
     <t>WindRejects</t>
   </si>
   <si>
-    <t>NE, SE</t>
-  </si>
-  <si>
     <t>SE, E</t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>SE, S</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -617,24 +578,9 @@
     <t>NW, W, SW, S</t>
   </si>
   <si>
-    <t>NW, NE, SE</t>
-  </si>
-  <si>
-    <t>N, S, SE</t>
-  </si>
-  <si>
-    <t>NW, N</t>
-  </si>
-  <si>
     <t>W, NW</t>
   </si>
   <si>
-    <t>SE, N</t>
-  </si>
-  <si>
-    <t>N, NW, W, SW, S</t>
-  </si>
-  <si>
     <t>NW</t>
   </si>
   <si>
@@ -644,48 +590,15 @@
     <t>W, S</t>
   </si>
   <si>
-    <t>W, SW, NE</t>
-  </si>
-  <si>
     <t>S, SW</t>
   </si>
   <si>
-    <t>W, NW, N</t>
-  </si>
-  <si>
-    <t>S, SW, W, NW</t>
-  </si>
-  <si>
-    <t>N, S, SW</t>
-  </si>
-  <si>
-    <t>N, E, S</t>
-  </si>
-  <si>
-    <t>SW, W, NW, N, NE</t>
-  </si>
-  <si>
     <t>NE</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>N, NE, E, SE, S, SW, W, NW</t>
-  </si>
-  <si>
-    <t>Might be outside the available domain</t>
-  </si>
-  <si>
-    <t>SW, S</t>
-  </si>
-  <si>
     <t>SE</t>
   </si>
   <si>
-    <t>W, E, NE</t>
-  </si>
-  <si>
     <t>SW</t>
   </si>
   <si>
@@ -711,6 +624,66 @@
   </si>
   <si>
     <t xml:space="preserve">    This handles the sign change at 180 deg, so e.g. [170, -170] excludes +/- 10 deg around 180 deg.</t>
+  </si>
+  <si>
+    <t>Baltimore, MD</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>Cheyenne, WY</t>
+  </si>
+  <si>
+    <t>Cheyenne</t>
+  </si>
+  <si>
+    <t>Austin, TX</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>[0.5 1 1 1]</t>
+  </si>
+  <si>
+    <t>[0.75 1 0.75 0.75]</t>
+  </si>
+  <si>
+    <t>[1 1 0.5 0.5]</t>
+  </si>
+  <si>
+    <t>S, SW, W</t>
+  </si>
+  <si>
+    <t>NW, SE</t>
+  </si>
+  <si>
+    <t>NE, W</t>
+  </si>
+  <si>
+    <t>E, SE, S</t>
+  </si>
+  <si>
+    <t>NW, W</t>
+  </si>
+  <si>
+    <t>S, SE, NW</t>
+  </si>
+  <si>
+    <t>E, SE, SW</t>
+  </si>
+  <si>
+    <t>W, NW, N, NE, E</t>
+  </si>
+  <si>
+    <t>NW, N, NE, SE</t>
+  </si>
+  <si>
+    <t>SE, NW</t>
+  </si>
+  <si>
+    <t>NE, SW</t>
   </si>
 </sst>
 </file>
@@ -766,8 +739,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -803,7 +778,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -815,6 +790,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -826,6 +802,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1155,19 +1132,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A56" sqref="A54:A56"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1184,13 +1163,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1206,11 +1185,14 @@
       <c r="E2">
         <v>30</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1227,984 +1209,1002 @@
         <v>35</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4">
+        <v>30.26</v>
+      </c>
+      <c r="D4">
+        <v>-97.74</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>35.299999999999997</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>-119</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>25</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="I4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="D6">
+        <v>-76.2</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>42.45</v>
       </c>
-      <c r="D5">
+      <c r="D7">
         <v>-71</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+      <c r="G7" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>35.25</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>-80.849999999999994</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>184</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+      <c r="F8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9">
+        <v>41.1</v>
+      </c>
+      <c r="D9">
+        <v>-104.8</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>41.8</v>
       </c>
-      <c r="D7">
+      <c r="D10">
         <v>-87.7</v>
       </c>
-      <c r="E7">
+      <c r="E10">
         <v>60</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C8">
+      <c r="C11">
         <v>39.1</v>
       </c>
-      <c r="D8">
+      <c r="D11">
         <v>-84.55</v>
       </c>
-      <c r="E8">
+      <c r="E11">
         <v>25</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
+      <c r="F11" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>41.45</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <v>-81.67</v>
-      </c>
-      <c r="E9">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10">
-        <v>40</v>
-      </c>
-      <c r="D10">
-        <v>-83.1</v>
-      </c>
-      <c r="E10">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11">
-        <v>32.85</v>
-      </c>
-      <c r="D11">
-        <v>-96.95</v>
-      </c>
-      <c r="E11">
-        <v>40</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>39.75</v>
-      </c>
-      <c r="D12">
-        <v>-105</v>
       </c>
       <c r="E12">
         <v>30</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="F12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>42.35</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>-83.1</v>
       </c>
       <c r="E13">
-        <v>45</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>30</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>36.700000000000003</v>
+        <v>32.85</v>
       </c>
       <c r="D14">
-        <v>-119.75</v>
+        <v>-96.95</v>
       </c>
       <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C15">
-        <v>29.8</v>
+        <v>39.75</v>
       </c>
       <c r="D15">
-        <v>-95.25</v>
+        <v>-105</v>
       </c>
       <c r="E15">
         <v>30</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C16">
-        <v>39.799999999999997</v>
+        <v>42.35</v>
       </c>
       <c r="D16">
-        <v>-86.15</v>
+        <v>-83.1</v>
       </c>
       <c r="E16">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:8">
+        <v>45</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C17">
-        <v>30.45</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="D17">
-        <v>-81.599999999999994</v>
+        <v>-119.75</v>
       </c>
       <c r="E17">
         <v>25</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="G17" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C18">
-        <v>39.15</v>
+        <v>29.8</v>
       </c>
       <c r="D18">
-        <v>-94.55</v>
+        <v>-95.25</v>
       </c>
       <c r="E18">
         <v>30</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C19">
-        <v>35.950000000000003</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="D19">
-        <v>-84</v>
+        <v>-86.15</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>175</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>171</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C20">
-        <v>36.200000000000003</v>
+        <v>30.45</v>
       </c>
       <c r="D20">
-        <v>-115.2</v>
+        <v>-81.599999999999994</v>
       </c>
       <c r="E20">
         <v>25</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="F20" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>39.15</v>
+      </c>
+      <c r="D21">
+        <v>-94.55</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="D22">
+        <v>-84</v>
+      </c>
+      <c r="E22">
+        <v>30</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D23">
+        <v>-115.2</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <v>34</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>-117.9</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <v>70</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C22">
+      <c r="C25">
         <v>35.1</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>-90.1</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>20</v>
       </c>
-      <c r="F22" t="s">
-        <v>167</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
+      <c r="F25" t="s">
+        <v>163</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C23">
+      <c r="C26">
         <v>26.05</v>
       </c>
-      <c r="D23">
+      <c r="D26">
         <v>-80.3</v>
       </c>
-      <c r="E23">
+      <c r="E26">
         <v>20</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="C24">
+      <c r="C27">
         <v>44.95</v>
       </c>
-      <c r="D24">
+      <c r="D27">
         <v>-93.25</v>
-      </c>
-      <c r="E24">
-        <v>30</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25">
-        <v>45.6</v>
-      </c>
-      <c r="D25">
-        <v>-73.7</v>
-      </c>
-      <c r="E25">
-        <v>30</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="D26">
-        <v>-86.6</v>
-      </c>
-      <c r="E26">
-        <v>30</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27">
-        <v>30.05</v>
-      </c>
-      <c r="D27">
-        <v>-90.3</v>
       </c>
       <c r="E27">
         <v>30</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C28">
-        <v>40.85</v>
+        <v>45.6</v>
       </c>
       <c r="D28">
         <v>-73.7</v>
       </c>
       <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="D29">
+        <v>-86.6</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30">
+        <v>30.05</v>
+      </c>
+      <c r="D30">
+        <v>-90.3</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31">
+        <v>40.85</v>
+      </c>
+      <c r="D31">
+        <v>-73.7</v>
+      </c>
+      <c r="E31">
         <v>70</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H28" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
+      <c r="G31" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="C29">
+      <c r="C32">
         <v>41.3</v>
       </c>
-      <c r="D29">
+      <c r="D32">
         <v>-96.05</v>
       </c>
-      <c r="E29">
+      <c r="E32">
         <v>25</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
+      <c r="F32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
         <v>61</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>62</v>
       </c>
-      <c r="C30">
+      <c r="C33">
         <v>28.5</v>
       </c>
-      <c r="D30">
+      <c r="D33">
         <v>-81.3</v>
       </c>
-      <c r="E30">
+      <c r="E33">
         <v>20</v>
       </c>
-      <c r="F30" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
+      <c r="F33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
         <v>63</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C31">
+      <c r="C34">
         <v>40</v>
       </c>
-      <c r="D31">
+      <c r="D34">
         <v>-75.2</v>
       </c>
-      <c r="E31">
+      <c r="E34">
         <v>50</v>
       </c>
-      <c r="F31" t="s">
-        <v>167</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H31" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
+      <c r="F34" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
         <v>65</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="C32">
+      <c r="C35">
         <v>33.6</v>
       </c>
-      <c r="D32">
+      <c r="D35">
         <v>-112</v>
       </c>
-      <c r="E32">
+      <c r="E35">
         <v>40</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
         <v>67</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>68</v>
       </c>
-      <c r="C33">
+      <c r="C36">
         <v>40.4</v>
       </c>
-      <c r="D33">
+      <c r="D36">
         <v>-79.95</v>
       </c>
-      <c r="E33">
+      <c r="E36">
         <v>25</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
+      <c r="G36" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
         <v>69</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
-      <c r="C34">
+      <c r="C37">
         <v>45.45</v>
       </c>
-      <c r="D34">
+      <c r="D37">
         <v>-122.55</v>
       </c>
-      <c r="E34">
+      <c r="E37">
         <v>30</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="C35">
+      <c r="C38">
         <v>39.549999999999997</v>
       </c>
-      <c r="D35">
+      <c r="D38">
         <v>-119.7</v>
-      </c>
-      <c r="E35">
-        <v>20</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15">
-      <c r="A36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36">
-        <v>37.4</v>
-      </c>
-      <c r="D36">
-        <v>-77.3</v>
-      </c>
-      <c r="E36">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
-        <v>164</v>
-      </c>
-      <c r="G36" s="2"/>
-      <c r="I36" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37">
-        <v>38.65</v>
-      </c>
-      <c r="D37">
-        <v>-121.4</v>
-      </c>
-      <c r="E37">
-        <v>25</v>
-      </c>
-      <c r="F37" t="s">
-        <v>164</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H37" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38">
-        <v>40.700000000000003</v>
-      </c>
-      <c r="D38">
-        <v>-111.95</v>
       </c>
       <c r="E38">
         <v>20</v>
       </c>
-      <c r="F38" t="s">
-        <v>175</v>
+      <c r="F38" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C39">
-        <v>29.55</v>
+        <v>37.4</v>
       </c>
       <c r="D39">
-        <v>-98.45</v>
+        <v>-77.3</v>
       </c>
       <c r="E39">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>167</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>160</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C40">
-        <v>32.799999999999997</v>
+        <v>38.65</v>
       </c>
       <c r="D40">
-        <v>-117</v>
+        <v>-121.4</v>
       </c>
       <c r="E40">
         <v>25</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="F40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="D41">
+        <v>-111.95</v>
+      </c>
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42">
+        <v>29.55</v>
+      </c>
+      <c r="D42">
+        <v>-98.45</v>
+      </c>
+      <c r="E42">
+        <v>30</v>
+      </c>
+      <c r="F42" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="D43">
+        <v>-117</v>
+      </c>
+      <c r="E43">
+        <v>25</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>84</v>
       </c>
-      <c r="C41">
+      <c r="C44">
         <v>37.6</v>
       </c>
-      <c r="D41">
+      <c r="D44">
         <v>-122</v>
       </c>
-      <c r="E41">
+      <c r="E44">
         <v>40</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" t="s">
+      <c r="G44" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>86</v>
       </c>
-      <c r="C42">
+      <c r="C45">
         <v>47.35</v>
       </c>
-      <c r="D42">
+      <c r="D45">
         <v>-122.25</v>
       </c>
-      <c r="E42">
+      <c r="E45">
         <v>50</v>
       </c>
-      <c r="F42" t="s">
-        <v>184</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
+      <c r="F45" t="s">
+        <v>174</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
         <v>87</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>88</v>
       </c>
-      <c r="C43">
+      <c r="C46">
         <v>38.65</v>
       </c>
-      <c r="D43">
+      <c r="D46">
         <v>-90.35</v>
       </c>
-      <c r="E43">
+      <c r="E46">
         <v>30</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" t="s">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
         <v>89</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>90</v>
       </c>
-      <c r="C44">
+      <c r="C47">
         <v>27.9</v>
       </c>
-      <c r="D44">
+      <c r="D47">
         <v>-82.4</v>
       </c>
-      <c r="E44">
+      <c r="E47">
         <v>30</v>
       </c>
-      <c r="F44" t="s">
-        <v>175</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
+      <c r="F47" t="s">
+        <v>171</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
         <v>91</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>92</v>
       </c>
-      <c r="C45">
+      <c r="C48">
         <v>43.7</v>
       </c>
-      <c r="D45">
+      <c r="D48">
         <v>-79.5</v>
       </c>
-      <c r="E45">
+      <c r="E48">
         <v>40</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G48" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49">
+        <v>32.25</v>
+      </c>
+      <c r="D49">
+        <v>-110.85</v>
+      </c>
+      <c r="E49">
+        <v>20</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50">
+        <v>38.9</v>
+      </c>
+      <c r="D50">
+        <v>-77</v>
+      </c>
+      <c r="E50">
+        <v>50</v>
+      </c>
+      <c r="F50" t="s">
+        <v>171</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46">
-        <v>32.25</v>
-      </c>
-      <c r="D46">
-        <v>-110.85</v>
-      </c>
-      <c r="E46">
-        <v>20</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C47">
-        <v>49.25</v>
-      </c>
-      <c r="D47">
-        <v>-122.85</v>
-      </c>
-      <c r="E47">
-        <v>25</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H47" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48">
-        <v>39.15</v>
-      </c>
-      <c r="D48">
-        <v>-76.8</v>
-      </c>
-      <c r="E48">
-        <v>50</v>
-      </c>
-      <c r="F48" t="s">
-        <v>175</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>228</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2224,14 +2224,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A32"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" customWidth="1"/>
   </cols>
@@ -2253,18 +2254,18 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>40.4</v>
@@ -2275,17 +2276,19 @@
       <c r="E2">
         <v>20</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="H2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>34.950000000000003</v>
@@ -2296,17 +2299,19 @@
       <c r="E3">
         <v>20</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="H3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>45.9</v>
@@ -2318,21 +2323,19 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>165</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>217</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C5">
         <v>40.1</v>
@@ -2343,17 +2346,19 @@
       <c r="E5">
         <v>20</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="H5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6">
         <v>34.549999999999997</v>
@@ -2364,17 +2369,19 @@
       <c r="E6">
         <v>20</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7">
         <v>40.5</v>
@@ -2387,15 +2394,15 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C8">
         <v>28.95</v>
@@ -2407,18 +2414,18 @@
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C9">
         <v>36.75</v>
@@ -2430,18 +2437,16 @@
         <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>165</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>204</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10">
         <v>40.549999999999997</v>
@@ -2453,18 +2458,18 @@
         <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="H10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C11">
         <v>37.950000000000003</v>
@@ -2475,19 +2480,19 @@
       <c r="E11">
         <v>20</v>
       </c>
-      <c r="F11" t="s">
-        <v>175</v>
+      <c r="F11" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12">
         <v>39.85</v>
@@ -2499,15 +2504,15 @@
         <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C13">
         <v>39.25</v>
@@ -2518,16 +2523,14 @@
       <c r="E13">
         <v>20</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14">
         <v>39.549999999999997</v>
@@ -2538,16 +2541,14 @@
       <c r="E14">
         <v>20</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>220</v>
-      </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C15">
         <v>41.75</v>
@@ -2558,19 +2559,17 @@
       <c r="E15">
         <v>20</v>
       </c>
-      <c r="F15" t="s">
-        <v>165</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>220</v>
-      </c>
+      <c r="F15" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C16">
         <v>39.85</v>
@@ -2582,18 +2581,18 @@
         <v>20</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C17">
         <v>36.049999999999997</v>
@@ -2604,17 +2603,19 @@
       <c r="E17">
         <v>20</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="H17" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C18">
         <v>37.200000000000003</v>
@@ -2626,15 +2627,15 @@
         <v>20</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19">
         <v>42.1</v>
@@ -2645,17 +2646,19 @@
       <c r="E19">
         <v>20</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="H19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C20">
         <v>47.4</v>
@@ -2666,136 +2669,110 @@
       <c r="E20">
         <v>35</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C21">
-        <v>35.6</v>
+        <v>36.9</v>
       </c>
       <c r="D21">
-        <v>-80.95</v>
+        <v>-111.35</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>187</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H21" t="s">
-        <v>166</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C22">
-        <v>36.9</v>
+        <v>29.8</v>
       </c>
       <c r="D22">
-        <v>-111.35</v>
+        <v>-81.55</v>
       </c>
       <c r="E22">
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="H22" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C23">
-        <v>29.8</v>
+        <v>40.9</v>
       </c>
       <c r="D23">
-        <v>-81.55</v>
+        <v>-117</v>
       </c>
       <c r="E23">
         <v>20</v>
       </c>
-      <c r="F23" t="s">
-        <v>187</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>143</v>
-      </c>
-      <c r="B24" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24">
-        <v>40.9</v>
-      </c>
-      <c r="D24">
-        <v>-117</v>
-      </c>
-      <c r="E24">
-        <v>20</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2840,18 +2817,18 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C2">
         <v>44.35</v>
@@ -2865,10 +2842,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C3">
         <v>29.25</v>
@@ -2882,10 +2859,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C4">
         <v>42.94</v>
@@ -2899,10 +2876,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C5">
         <v>36.24</v>
@@ -2916,10 +2893,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C6">
         <v>36.06</v>
@@ -2933,10 +2910,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C7">
         <v>35.68</v>
@@ -2950,10 +2927,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C8">
         <v>34.51</v>
@@ -2967,10 +2944,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C9">
         <v>48.1</v>
@@ -2984,10 +2961,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C10">
         <v>43.87</v>
@@ -3001,10 +2978,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C11">
         <v>35.07</v>
@@ -3018,10 +2995,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C12">
         <v>33</v>
@@ -3035,10 +3012,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C13">
         <v>38.53</v>
@@ -3052,10 +3029,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C14">
         <v>44.6</v>
@@ -3069,10 +3046,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C15">
         <v>37.83</v>
@@ -3086,10 +3063,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C16">
         <v>37.299999999999997</v>

</xml_diff>

<commit_message>
Added NE and SW to Philadelphia wind reject directions
</commit_message>
<xml_diff>
--- a/Workspaces/SiteData/trend_locations.xlsx
+++ b/Workspaces/SiteData/trend_locations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="223">
   <si>
     <t>Location</t>
   </si>
@@ -690,6 +690,9 @@
   </si>
   <si>
     <t>E, SW, N</t>
+  </si>
+  <si>
+    <t>SW, NE</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1148,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1850,7 +1853,9 @@
       <c r="F34" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">

</xml_diff>